<commit_message>
Updated Mockups and FP
</commit_message>
<xml_diff>
--- a/FP UC/fp.xlsx
+++ b/FP UC/fp.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Stunden</t>
   </si>
@@ -58,12 +58,15 @@
   <si>
     <t>Upload Image</t>
   </si>
+  <si>
+    <t>NEW</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +77,13 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,11 +136,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -581,7 +594,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1474,10 +1487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1532,35 +1545,35 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>24.7</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="5">
         <v>21.45</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="5">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="4">
         <v>20.28</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>11</v>
       </c>
     </row>
@@ -1584,6 +1597,11 @@
       </c>
       <c r="C9" s="3">
         <v>6.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Attributes and FP Excel
</commit_message>
<xml_diff>
--- a/FP UC/fp.xlsx
+++ b/FP UC/fp.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>Stunden</t>
   </si>
@@ -60,6 +60,66 @@
   </si>
   <si>
     <t>Attributes</t>
+  </si>
+  <si>
+    <t>UC</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>18h</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>25h</t>
+  </si>
+  <si>
+    <t>5h</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>23h</t>
+  </si>
+  <si>
+    <t>31h</t>
+  </si>
+  <si>
+    <t>0,5h</t>
+  </si>
+  <si>
+    <t>6,5h</t>
+  </si>
+  <si>
+    <t>6h</t>
+  </si>
+  <si>
+    <t>8h</t>
+  </si>
+  <si>
+    <t>12h</t>
+  </si>
+  <si>
+    <t>14h</t>
   </si>
 </sst>
 </file>
@@ -91,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,6 +167,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -151,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -160,6 +226,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1629,10 +1696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1748,6 +1815,131 @@
         <v>11</v>
       </c>
     </row>
+    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="1">
+        <f>B3</f>
+        <v>23.45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="2">
+        <f>B2</f>
+        <v>51.48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="1">
+        <f>B6</f>
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="2">
+        <f>B5</f>
+        <v>13.26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="1">
+        <f>B4</f>
+        <v>17.940000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>